<commit_message>
Update DD effort spent and GANTT
</commit_message>
<xml_diff>
--- a/DD/GANTT.xlsx
+++ b/DD/GANTT.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="432" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>WHO</t>
   </si>
@@ -66,12 +66,21 @@
   </si>
   <si>
     <t>Architectural Design G</t>
+  </si>
+  <si>
+    <t>API Manager Implementation</t>
+  </si>
+  <si>
+    <t>Data Layer Implementation</t>
+  </si>
+  <si>
+    <t>Java Class Structure Building</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,14 +457,14 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="32" width="3.6640625" customWidth="1"/>
+    <col min="3" max="32" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
@@ -699,12 +708,44 @@
       <c r="AF11" s="2"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
       <c r="AF12" s="2"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
       <c r="AF13" s="2"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
       <c r="AF14" s="2"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
@@ -746,7 +787,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -758,7 +799,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementation, integration and test Plan
</commit_message>
<xml_diff>
--- a/DD/GANTT.xlsx
+++ b/DD/GANTT.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiadifatta/Documents/GitHub/BiasielliCapoDifatta/DD/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14600"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -18,9 +13,6 @@
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>WHO</t>
   </si>
@@ -82,7 +74,13 @@
     <t>Data Layer Implementation</t>
   </si>
   <si>
-    <t>Java Class Structure Building</t>
+    <t>Java Class Structure Building (controller)</t>
+  </si>
+  <si>
+    <t>REQUIREMENTS TRACEABILITY</t>
+  </si>
+  <si>
+    <t>IMPLEMENTATION, INTEGRATION AND TEST PLAN</t>
   </si>
 </sst>
 </file>
@@ -168,7 +166,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -473,14 +471,14 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="32" width="3.6640625" customWidth="1"/>
+    <col min="3" max="32" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
@@ -717,10 +715,10 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
       <c r="AF11" s="2"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
@@ -743,11 +741,11 @@
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
       <c r="AF13" s="2"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
@@ -757,17 +755,35 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
       <c r="AF14" s="2"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
       <c r="AF15" s="2"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
       <c r="AF16" s="2"/>
     </row>
     <row r="17" spans="32:32" x14ac:dyDescent="0.2">
@@ -803,7 +819,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -815,7 +831,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>